<commit_message>
pre alfa, se puede asignar prioridad a los ramos y a las secciones, se muestra todas las opciones y la de mayor peso, limitado a 6 ramos por semestre
</commit_message>
<xml_diff>
--- a/RutaCritica/MallaCurricular.xlsx
+++ b/RutaCritica/MallaCurricular.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Flores\Desktop\grafos\Proyecto semestral\recomendador-de-horarios-UDP\generador_de_horarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Flores\Desktop\practica II 2021\generador_de_horarios_Practica\RutaCritica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA848DA6-8614-4BD8-89F6-0E4F88CB868B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DB4E39F-2574-43CD-912A-435720079E76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{4E8A2F0A-3134-4A00-A9B2-0591E032DEE3}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="130">
   <si>
     <t>CBM1000</t>
   </si>
@@ -149,9 +149,6 @@
     <t>CIT2201</t>
   </si>
   <si>
-    <t>Electivo Profesional</t>
-  </si>
-  <si>
     <t>CIT33XX-1</t>
   </si>
   <si>
@@ -227,9 +224,6 @@
     <t>34, 41</t>
   </si>
   <si>
-    <t>31, 35</t>
-  </si>
-  <si>
     <t>39, 41</t>
   </si>
   <si>
@@ -402,6 +396,33 @@
   </si>
   <si>
     <t xml:space="preserve">3, 10, 13 , 17, 20, 26, 27, 28, 29, 36, 37, 38, 39, 40, 42, 43, 44, 45, 47, 48, 49, 50, 51, 52 </t>
+  </si>
+  <si>
+    <t>31, 34</t>
+  </si>
+  <si>
+    <t>Electivo Profesional-1</t>
+  </si>
+  <si>
+    <t>Electivo Profesional-2</t>
+  </si>
+  <si>
+    <t>Electivo Profesional-3</t>
+  </si>
+  <si>
+    <t>Electivo Profesional-4</t>
+  </si>
+  <si>
+    <t>Electivo Profesional-5</t>
+  </si>
+  <si>
+    <t>Electivo Profesional-6</t>
+  </si>
+  <si>
+    <t>Electivo Profesional-7</t>
+  </si>
+  <si>
+    <t>Electivo Profesional-8</t>
   </si>
 </sst>
 </file>
@@ -947,8 +968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC6E64A-71CB-4B98-A7E7-F4D52075C1FC}">
   <dimension ref="A2:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="J44" sqref="J44"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,19 +984,19 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>51</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -986,10 +1007,10 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E3" s="21">
         <v>1</v>
@@ -1006,10 +1027,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E4" s="21">
         <v>1</v>
@@ -1026,10 +1047,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E5" s="21">
         <v>1</v>
@@ -1046,7 +1067,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D6" s="12">
         <v>9</v>
@@ -1066,7 +1087,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D7" s="12">
         <v>38</v>
@@ -1086,10 +1107,10 @@
         <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E8" s="22">
         <v>2</v>
@@ -1106,10 +1127,10 @@
         <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E9" s="22">
         <v>2</v>
@@ -1126,10 +1147,10 @@
         <v>7</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E10" s="22">
         <v>2</v>
@@ -1146,10 +1167,10 @@
         <v>8</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E11" s="22">
         <v>2</v>
@@ -1163,13 +1184,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E12" s="22">
         <v>2</v>
@@ -1186,7 +1207,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D13" s="14">
         <v>18</v>
@@ -1195,7 +1216,7 @@
         <v>3</v>
       </c>
       <c r="F13" s="32" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1206,10 +1227,10 @@
         <v>10</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E14" s="23">
         <v>3</v>
@@ -1226,16 +1247,16 @@
         <v>11</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E15" s="23">
         <v>3</v>
       </c>
       <c r="F15" s="32" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1246,7 +1267,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D16" s="14">
         <v>19</v>
@@ -1266,10 +1287,10 @@
         <v>13</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E17" s="23">
         <v>3</v>
@@ -1286,16 +1307,16 @@
         <v>14</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E18" s="24">
         <v>4</v>
       </c>
       <c r="F18" s="32" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1306,16 +1327,16 @@
         <v>15</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E19" s="24">
         <v>4</v>
       </c>
       <c r="F19" s="32" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1326,7 +1347,7 @@
         <v>16</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D20" s="15">
         <v>23</v>
@@ -1335,7 +1356,7 @@
         <v>4</v>
       </c>
       <c r="F20" s="32" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1346,10 +1367,10 @@
         <v>17</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E21" s="24">
         <v>4</v>
@@ -1363,13 +1384,13 @@
         <v>20</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E22" s="24">
         <v>4</v>
@@ -1386,7 +1407,7 @@
         <v>18</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D23" s="15">
         <v>27</v>
@@ -1406,7 +1427,7 @@
         <v>19</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D24" s="16">
         <v>29</v>
@@ -1415,7 +1436,7 @@
         <v>5</v>
       </c>
       <c r="F24" s="32" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1426,10 +1447,10 @@
         <v>20</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D25" s="38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E25" s="25">
         <v>5</v>
@@ -1446,16 +1467,16 @@
         <v>21</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E26" s="25">
         <v>5</v>
       </c>
       <c r="F26" s="32" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -1466,10 +1487,10 @@
         <v>22</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>64</v>
+        <v>121</v>
       </c>
       <c r="E27" s="25">
         <v>5</v>
@@ -1483,13 +1504,13 @@
         <v>26</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E28" s="25">
         <v>5</v>
@@ -1506,10 +1527,10 @@
         <v>23</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E29" s="25">
         <v>5</v>
@@ -1527,10 +1548,10 @@
         <v>24</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E30" s="26">
         <v>6</v>
@@ -1547,16 +1568,16 @@
         <v>25</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E31" s="26">
         <v>6</v>
       </c>
       <c r="F31" s="34" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -1567,7 +1588,7 @@
         <v>26</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D32" s="17">
         <v>35</v>
@@ -1576,7 +1597,7 @@
         <v>6</v>
       </c>
       <c r="F32" s="32" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1587,7 +1608,7 @@
         <v>27</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D33" s="17">
         <v>40</v>
@@ -1596,7 +1617,7 @@
         <v>6</v>
       </c>
       <c r="F33" s="32" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1607,7 +1628,7 @@
         <v>28</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D34" s="17">
         <v>37</v>
@@ -1627,7 +1648,7 @@
         <v>29</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D35" s="18">
         <v>46</v>
@@ -1647,16 +1668,16 @@
         <v>30</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E36" s="27">
         <v>7</v>
       </c>
       <c r="F36" s="32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1667,7 +1688,7 @@
         <v>31</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D37" s="18">
         <v>41</v>
@@ -1687,10 +1708,10 @@
         <v>32</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E38" s="27">
         <v>7</v>
@@ -1707,10 +1728,10 @@
         <v>33</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E39" s="27">
         <v>7</v>
@@ -1727,10 +1748,10 @@
         <v>34</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E40" s="28">
         <v>8</v>
@@ -1747,10 +1768,10 @@
         <v>35</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E41" s="28">
         <v>8</v>
@@ -1767,10 +1788,10 @@
         <v>36</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E42" s="28">
         <v>8</v>
@@ -1787,7 +1808,7 @@
         <v>37</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D43" s="19">
         <v>46</v>
@@ -1796,7 +1817,7 @@
         <v>8</v>
       </c>
       <c r="F43" s="33" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1804,13 +1825,13 @@
         <v>42</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D44" s="19" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E44" s="28">
         <v>8</v>
@@ -1824,13 +1845,13 @@
         <v>43</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>38</v>
+        <v>122</v>
       </c>
       <c r="D45" s="20" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E45" s="29">
         <v>9</v>
@@ -1844,13 +1865,13 @@
         <v>44</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>38</v>
+        <v>123</v>
       </c>
       <c r="D46" s="20" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E46" s="29">
         <v>9</v>
@@ -1864,13 +1885,13 @@
         <v>45</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>38</v>
+        <v>124</v>
       </c>
       <c r="D47" s="20" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E47" s="29">
         <v>9</v>
@@ -1884,10 +1905,10 @@
         <v>46</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D48" s="20">
         <v>51</v>
@@ -1896,7 +1917,7 @@
         <v>9</v>
       </c>
       <c r="F48" s="32" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -1904,13 +1925,13 @@
         <v>47</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>38</v>
+        <v>125</v>
       </c>
       <c r="D49" s="20" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E49" s="29">
         <v>9</v>
@@ -1924,13 +1945,13 @@
         <v>48</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>38</v>
+        <v>126</v>
       </c>
       <c r="D50" s="39" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E50" s="30">
         <v>10</v>
@@ -1944,13 +1965,13 @@
         <v>49</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>38</v>
+        <v>127</v>
       </c>
       <c r="D51" s="39" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E51" s="30">
         <v>10</v>
@@ -1964,13 +1985,13 @@
         <v>50</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>38</v>
+        <v>128</v>
       </c>
       <c r="D52" s="39" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E52" s="30">
         <v>10</v>
@@ -1984,13 +2005,13 @@
         <v>51</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D53" s="39" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E53" s="30">
         <v>10</v>
@@ -2004,13 +2025,13 @@
         <v>52</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>38</v>
+        <v>129</v>
       </c>
       <c r="D54" s="39" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E54" s="30">
         <v>10</v>
@@ -2024,10 +2045,10 @@
         <v>53</v>
       </c>
       <c r="B55" s="35" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C55" s="35" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D55" s="40">
         <v>0</v>
@@ -2036,7 +2057,7 @@
         <v>11</v>
       </c>
       <c r="F55" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "pre alfa, se puede asignar prioridad a los ramos y a las secciones, se muestra todas las opciones y la de mayor peso, limitado a 6 ramos por semestre"
This reverts commit bd35fa0d6d6ece96ad9bb7c9f3a251812857c020.
</commit_message>
<xml_diff>
--- a/RutaCritica/MallaCurricular.xlsx
+++ b/RutaCritica/MallaCurricular.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Flores\Desktop\practica II 2021\generador_de_horarios_Practica\RutaCritica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Flores\Desktop\grafos\Proyecto semestral\recomendador-de-horarios-UDP\generador_de_horarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DB4E39F-2574-43CD-912A-435720079E76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA848DA6-8614-4BD8-89F6-0E4F88CB868B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{4E8A2F0A-3134-4A00-A9B2-0591E032DEE3}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="123">
   <si>
     <t>CBM1000</t>
   </si>
@@ -149,6 +149,9 @@
     <t>CIT2201</t>
   </si>
   <si>
+    <t>Electivo Profesional</t>
+  </si>
+  <si>
     <t>CIT33XX-1</t>
   </si>
   <si>
@@ -224,6 +227,9 @@
     <t>34, 41</t>
   </si>
   <si>
+    <t>31, 35</t>
+  </si>
+  <si>
     <t>39, 41</t>
   </si>
   <si>
@@ -396,33 +402,6 @@
   </si>
   <si>
     <t xml:space="preserve">3, 10, 13 , 17, 20, 26, 27, 28, 29, 36, 37, 38, 39, 40, 42, 43, 44, 45, 47, 48, 49, 50, 51, 52 </t>
-  </si>
-  <si>
-    <t>31, 34</t>
-  </si>
-  <si>
-    <t>Electivo Profesional-1</t>
-  </si>
-  <si>
-    <t>Electivo Profesional-2</t>
-  </si>
-  <si>
-    <t>Electivo Profesional-3</t>
-  </si>
-  <si>
-    <t>Electivo Profesional-4</t>
-  </si>
-  <si>
-    <t>Electivo Profesional-5</t>
-  </si>
-  <si>
-    <t>Electivo Profesional-6</t>
-  </si>
-  <si>
-    <t>Electivo Profesional-7</t>
-  </si>
-  <si>
-    <t>Electivo Profesional-8</t>
   </si>
 </sst>
 </file>
@@ -968,8 +947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC6E64A-71CB-4B98-A7E7-F4D52075C1FC}">
   <dimension ref="A2:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,19 +963,19 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>49</v>
-      </c>
       <c r="D2" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>52</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1007,10 +986,10 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E3" s="21">
         <v>1</v>
@@ -1027,10 +1006,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E4" s="21">
         <v>1</v>
@@ -1047,10 +1026,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E5" s="21">
         <v>1</v>
@@ -1067,7 +1046,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D6" s="12">
         <v>9</v>
@@ -1087,7 +1066,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D7" s="12">
         <v>38</v>
@@ -1107,10 +1086,10 @@
         <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E8" s="22">
         <v>2</v>
@@ -1127,10 +1106,10 @@
         <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E9" s="22">
         <v>2</v>
@@ -1147,10 +1126,10 @@
         <v>7</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E10" s="22">
         <v>2</v>
@@ -1167,10 +1146,10 @@
         <v>8</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E11" s="22">
         <v>2</v>
@@ -1184,13 +1163,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E12" s="22">
         <v>2</v>
@@ -1207,7 +1186,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D13" s="14">
         <v>18</v>
@@ -1216,7 +1195,7 @@
         <v>3</v>
       </c>
       <c r="F13" s="32" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1227,10 +1206,10 @@
         <v>10</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E14" s="23">
         <v>3</v>
@@ -1247,16 +1226,16 @@
         <v>11</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E15" s="23">
         <v>3</v>
       </c>
       <c r="F15" s="32" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1267,7 +1246,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D16" s="14">
         <v>19</v>
@@ -1287,10 +1266,10 @@
         <v>13</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E17" s="23">
         <v>3</v>
@@ -1307,16 +1286,16 @@
         <v>14</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E18" s="24">
         <v>4</v>
       </c>
       <c r="F18" s="32" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1327,16 +1306,16 @@
         <v>15</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E19" s="24">
         <v>4</v>
       </c>
       <c r="F19" s="32" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1347,7 +1326,7 @@
         <v>16</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D20" s="15">
         <v>23</v>
@@ -1356,7 +1335,7 @@
         <v>4</v>
       </c>
       <c r="F20" s="32" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1367,10 +1346,10 @@
         <v>17</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E21" s="24">
         <v>4</v>
@@ -1384,13 +1363,13 @@
         <v>20</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E22" s="24">
         <v>4</v>
@@ -1407,7 +1386,7 @@
         <v>18</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D23" s="15">
         <v>27</v>
@@ -1427,7 +1406,7 @@
         <v>19</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D24" s="16">
         <v>29</v>
@@ -1436,7 +1415,7 @@
         <v>5</v>
       </c>
       <c r="F24" s="32" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1447,10 +1426,10 @@
         <v>20</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D25" s="38" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E25" s="25">
         <v>5</v>
@@ -1467,16 +1446,16 @@
         <v>21</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E26" s="25">
         <v>5</v>
       </c>
       <c r="F26" s="32" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -1487,10 +1466,10 @@
         <v>22</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>121</v>
+        <v>64</v>
       </c>
       <c r="E27" s="25">
         <v>5</v>
@@ -1504,13 +1483,13 @@
         <v>26</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E28" s="25">
         <v>5</v>
@@ -1527,10 +1506,10 @@
         <v>23</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E29" s="25">
         <v>5</v>
@@ -1548,10 +1527,10 @@
         <v>24</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E30" s="26">
         <v>6</v>
@@ -1568,16 +1547,16 @@
         <v>25</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E31" s="26">
         <v>6</v>
       </c>
       <c r="F31" s="34" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -1588,7 +1567,7 @@
         <v>26</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D32" s="17">
         <v>35</v>
@@ -1597,7 +1576,7 @@
         <v>6</v>
       </c>
       <c r="F32" s="32" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1608,7 +1587,7 @@
         <v>27</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D33" s="17">
         <v>40</v>
@@ -1617,7 +1596,7 @@
         <v>6</v>
       </c>
       <c r="F33" s="32" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1628,7 +1607,7 @@
         <v>28</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D34" s="17">
         <v>37</v>
@@ -1648,7 +1627,7 @@
         <v>29</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D35" s="18">
         <v>46</v>
@@ -1668,16 +1647,16 @@
         <v>30</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E36" s="27">
         <v>7</v>
       </c>
       <c r="F36" s="32" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1688,7 +1667,7 @@
         <v>31</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D37" s="18">
         <v>41</v>
@@ -1708,10 +1687,10 @@
         <v>32</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E38" s="27">
         <v>7</v>
@@ -1728,10 +1707,10 @@
         <v>33</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E39" s="27">
         <v>7</v>
@@ -1748,10 +1727,10 @@
         <v>34</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E40" s="28">
         <v>8</v>
@@ -1768,10 +1747,10 @@
         <v>35</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E41" s="28">
         <v>8</v>
@@ -1788,10 +1767,10 @@
         <v>36</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E42" s="28">
         <v>8</v>
@@ -1808,7 +1787,7 @@
         <v>37</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D43" s="19">
         <v>46</v>
@@ -1817,7 +1796,7 @@
         <v>8</v>
       </c>
       <c r="F43" s="33" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1825,13 +1804,13 @@
         <v>42</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D44" s="19" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E44" s="28">
         <v>8</v>
@@ -1845,13 +1824,13 @@
         <v>43</v>
       </c>
       <c r="B45" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C45" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C45" s="9" t="s">
-        <v>122</v>
-      </c>
       <c r="D45" s="20" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E45" s="29">
         <v>9</v>
@@ -1865,13 +1844,13 @@
         <v>44</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>123</v>
+        <v>38</v>
       </c>
       <c r="D46" s="20" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E46" s="29">
         <v>9</v>
@@ -1885,13 +1864,13 @@
         <v>45</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>124</v>
+        <v>38</v>
       </c>
       <c r="D47" s="20" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E47" s="29">
         <v>9</v>
@@ -1905,10 +1884,10 @@
         <v>46</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D48" s="20">
         <v>51</v>
@@ -1917,7 +1896,7 @@
         <v>9</v>
       </c>
       <c r="F48" s="32" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -1925,13 +1904,13 @@
         <v>47</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>125</v>
+        <v>38</v>
       </c>
       <c r="D49" s="20" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E49" s="29">
         <v>9</v>
@@ -1945,13 +1924,13 @@
         <v>48</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>126</v>
+        <v>38</v>
       </c>
       <c r="D50" s="39" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E50" s="30">
         <v>10</v>
@@ -1965,13 +1944,13 @@
         <v>49</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>127</v>
+        <v>38</v>
       </c>
       <c r="D51" s="39" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E51" s="30">
         <v>10</v>
@@ -1985,13 +1964,13 @@
         <v>50</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>128</v>
+        <v>38</v>
       </c>
       <c r="D52" s="39" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E52" s="30">
         <v>10</v>
@@ -2005,13 +1984,13 @@
         <v>51</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D53" s="39" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E53" s="30">
         <v>10</v>
@@ -2025,13 +2004,13 @@
         <v>52</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>129</v>
+        <v>38</v>
       </c>
       <c r="D54" s="39" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E54" s="30">
         <v>10</v>
@@ -2045,10 +2024,10 @@
         <v>53</v>
       </c>
       <c r="B55" s="35" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C55" s="35" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D55" s="40">
         <v>0</v>
@@ -2057,7 +2036,7 @@
         <v>11</v>
       </c>
       <c r="F55" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>